<commit_message>
1) Reordered sector overview and detail 2) Included Summary and Detail in always/high_materiality sector scenario layout
</commit_message>
<xml_diff>
--- a/src/assets/config/config.xlsx
+++ b/src/assets/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\cfrf_tool\dash_tool\src\assets\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F880BF3D-881A-4375-A587-76D20D68B8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D512F4E-6E61-4152-BCE1-FD86E1030E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5B5ABE24-C80C-4D95-A370-49246C7988A0}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5B5ABE24-C80C-4D95-A370-49246C7988A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Output Structure Mapping" sheetId="5" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Output Structure Mapping'!$A$1:$H$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -491,34 +492,34 @@
     <t>sovereigns/country/bra_sov</t>
   </si>
   <si>
-    <t>underwritng/aviation</t>
-  </si>
-  <si>
-    <t>underwritng/casualty</t>
-  </si>
-  <si>
-    <t>underwritng/energy</t>
-  </si>
-  <si>
-    <t>underwritng/life_protection</t>
-  </si>
-  <si>
-    <t>underwritng/savings_and_retirement</t>
-  </si>
-  <si>
-    <t>underwritng/health</t>
-  </si>
-  <si>
-    <t>underwritng/marine</t>
-  </si>
-  <si>
-    <t>underwritng/property</t>
-  </si>
-  <si>
-    <t>underwritng/motor</t>
-  </si>
-  <si>
     <t>sovereigns</t>
+  </si>
+  <si>
+    <t>underwriting/life_protection</t>
+  </si>
+  <si>
+    <t>underwriting/savings_and_retirement</t>
+  </si>
+  <si>
+    <t>underwriting/health</t>
+  </si>
+  <si>
+    <t>underwriting/aviation</t>
+  </si>
+  <si>
+    <t>underwriting/casualty</t>
+  </si>
+  <si>
+    <t>underwriting/energy</t>
+  </si>
+  <si>
+    <t>underwriting/marine</t>
+  </si>
+  <si>
+    <t>underwriting/motor</t>
+  </si>
+  <si>
+    <t>underwriting/property</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1042,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:G17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1638,7 +1639,7 @@
   <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:F48"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2518,7 +2519,7 @@
         <v>138</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>69</v>
@@ -2541,7 +2542,7 @@
         <v>139</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>69</v>
@@ -2564,7 +2565,7 @@
         <v>140</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>69</v>
@@ -2587,7 +2588,7 @@
         <v>141</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>69</v>
@@ -2610,7 +2611,7 @@
         <v>142</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>69</v>
@@ -2633,7 +2634,7 @@
         <v>143</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>69</v>
@@ -2656,7 +2657,7 @@
         <v>144</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>69</v>
@@ -2679,7 +2680,7 @@
         <v>145</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>69</v>
@@ -2702,7 +2703,7 @@
         <v>146</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>69</v>
@@ -2725,7 +2726,7 @@
         <v>147</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>69</v>
@@ -2748,7 +2749,7 @@
         <v>148</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>69</v>
@@ -2768,7 +2769,7 @@
         <v>31</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>83</v>
@@ -2791,7 +2792,7 @@
         <v>31</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>83</v>
@@ -2814,7 +2815,7 @@
         <v>31</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>83</v>
@@ -2837,7 +2838,7 @@
         <v>31</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>88</v>
@@ -2860,7 +2861,7 @@
         <v>31</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>88</v>
@@ -2883,7 +2884,7 @@
         <v>31</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>88</v>
@@ -2906,7 +2907,7 @@
         <v>31</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>88</v>
@@ -2952,7 +2953,7 @@
         <v>31</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>88</v>
@@ -4163,6 +4164,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e0782aab-51b8-4ca3-98ff-55b4e7f68941" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="33eab63c-ae56-4068-bee3-9f3b1109b8c5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009D19F62891C3BD42A3B191BFE4257989" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f702a18db7d267400f964a70eb93e56">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="33eab63c-ae56-4068-bee3-9f3b1109b8c5" xmlns:ns3="e0782aab-51b8-4ca3-98ff-55b4e7f68941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15fa389961bd8124ae695162c3af3829" ns2:_="" ns3:_="">
     <xsd:import namespace="33eab63c-ae56-4068-bee3-9f3b1109b8c5"/>
@@ -4411,41 +4432,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e0782aab-51b8-4ca3-98ff-55b4e7f68941" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="33eab63c-ae56-4068-bee3-9f3b1109b8c5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{687CEDA3-8ED7-4B9A-8A23-5EF152B8A1F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CE1014F-E953-4C02-A404-BD3BED220A6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="33eab63c-ae56-4068-bee3-9f3b1109b8c5"/>
-    <ds:schemaRef ds:uri="e0782aab-51b8-4ca3-98ff-55b4e7f68941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4468,9 +4458,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CE1014F-E953-4C02-A404-BD3BED220A6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{687CEDA3-8ED7-4B9A-8A23-5EF152B8A1F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="33eab63c-ae56-4068-bee3-9f3b1109b8c5"/>
+    <ds:schemaRef ds:uri="e0782aab-51b8-4ca3-98ff-55b4e7f68941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Customisation of scenario report, enhancements of links between pages in reports
</commit_message>
<xml_diff>
--- a/src/assets/config/config.xlsx
+++ b/src/assets/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\cfrf_tool\dash_tool\src\assets\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E25E8E4B-69EB-425E-A50C-D6D511D6238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AADF12-5956-4A58-B822-20B98CE78CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5B5ABE24-C80C-4D95-A370-49246C7988A0}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5B5ABE24-C80C-4D95-A370-49246C7988A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Output Structure Mapping" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Exposure-Sector-Product Mapping" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Exposure-Sector-Product Mapping'!$A$1:$F$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Exposure-Sector-Product Mapping'!$A$1:$F$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Output Structure Mapping'!$A$1:$H$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1516,8 +1516,8 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1610,8 +1610,8 @@
   </sheetPr>
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G39" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1620,7 +1620,8 @@
     <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -2365,222 +2366,222 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>148</v>
+        <v>75</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>148</v>
+        <v>75</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>148</v>
+        <v>75</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>138</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>138</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -2588,19 +2589,19 @@
         <v>74</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -2608,19 +2609,19 @@
         <v>74</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -2628,19 +2629,19 @@
         <v>74</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -2648,19 +2649,19 @@
         <v>74</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -2668,19 +2669,19 @@
         <v>74</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -2688,19 +2689,19 @@
         <v>74</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -2708,19 +2709,19 @@
         <v>74</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -2728,19 +2729,19 @@
         <v>74</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -2748,19 +2749,19 @@
         <v>74</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -2771,16 +2772,16 @@
         <v>88</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -2791,16 +2792,16 @@
         <v>88</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -2811,16 +2812,16 @@
         <v>88</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -2831,16 +2832,16 @@
         <v>88</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -2851,16 +2852,16 @@
         <v>88</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -2871,16 +2872,16 @@
         <v>88</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -2891,16 +2892,16 @@
         <v>88</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -2911,16 +2912,16 @@
         <v>88</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -2931,16 +2932,16 @@
         <v>88</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -2948,16 +2949,16 @@
         <v>74</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>53</v>
@@ -2968,16 +2969,16 @@
         <v>74</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>47</v>
@@ -2988,19 +2989,19 @@
         <v>74</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -3008,176 +3009,176 @@
         <v>74</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>53</v>
@@ -3185,62 +3186,62 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
@@ -3251,16 +3252,16 @@
         <v>88</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
@@ -3271,16 +3272,16 @@
         <v>88</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -3291,16 +3292,16 @@
         <v>88</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
@@ -3311,16 +3312,16 @@
         <v>88</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
@@ -3331,16 +3332,16 @@
         <v>88</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
@@ -3351,16 +3352,16 @@
         <v>88</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
@@ -3371,16 +3372,16 @@
         <v>88</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
@@ -3391,16 +3392,16 @@
         <v>88</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -3411,16 +3412,16 @@
         <v>88</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -3428,19 +3429,19 @@
         <v>95</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -3448,19 +3449,19 @@
         <v>95</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -3468,19 +3469,19 @@
         <v>95</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -3488,19 +3489,19 @@
         <v>95</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -3508,19 +3509,19 @@
         <v>95</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -3528,19 +3529,19 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -3548,19 +3549,19 @@
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
@@ -3568,239 +3569,239 @@
         <v>95</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Selection of sector report
</commit_message>
<xml_diff>
--- a/src/assets/config/config.xlsx
+++ b/src/assets/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\cfrf_tool\dash_tool\src\assets\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AADF12-5956-4A58-B822-20B98CE78CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65F5D44-9A4C-4111-9BCA-4B84C296E80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5B5ABE24-C80C-4D95-A370-49246C7988A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5B5ABE24-C80C-4D95-A370-49246C7988A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Output Structure Mapping" sheetId="5" r:id="rId1"/>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1610,8 +1610,8 @@
   </sheetPr>
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixes to sector report
</commit_message>
<xml_diff>
--- a/src/assets/config/config.xlsx
+++ b/src/assets/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\cfrf_tool\dash_tool\src\assets\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65F5D44-9A4C-4111-9BCA-4B84C296E80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F9FFB2-4E1E-48EF-8559-7064B049EDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5B5ABE24-C80C-4D95-A370-49246C7988A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5B5ABE24-C80C-4D95-A370-49246C7988A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Output Structure Mapping" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Exposure-Sector-Product Mapping'!$A$1:$F$98</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Output Structure Mapping'!$A$1:$H$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Output Structure Mapping'!$A$1:$H$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="149">
   <si>
     <t>Output Structure</t>
   </si>
@@ -348,9 +348,6 @@
   </si>
   <si>
     <t>Scenario</t>
-  </si>
-  <si>
-    <t>Full</t>
   </si>
   <si>
     <t>Disorderly Scenario</t>
@@ -546,7 +543,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -634,21 +631,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -659,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -672,9 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,10 +992,10 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1047,10 +1027,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -1201,7 +1181,7 @@
         <v>97</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>11</v>
@@ -1209,7 +1189,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1219,7 +1199,7 @@
         <v>97</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>11</v>
@@ -1227,66 +1207,66 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="14"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
@@ -1329,7 +1309,7 @@
         <v>100</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>11</v>
@@ -1337,7 +1317,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -1347,7 +1327,7 @@
         <v>100</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>11</v>
@@ -1355,7 +1335,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -1396,114 +1376,7 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
+    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1544,7 +1417,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
@@ -1558,7 +1431,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>21</v>
@@ -1572,7 +1445,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
@@ -1586,7 +1459,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>28</v>
@@ -1610,7 +1483,7 @@
   </sheetPr>
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+    <sheetView topLeftCell="A74" workbookViewId="0">
       <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
@@ -1638,7 +1511,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>33</v>
@@ -1658,7 +1531,7 @@
         <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>38</v>
@@ -1678,7 +1551,7 @@
         <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>38</v>
@@ -1698,7 +1571,7 @@
         <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>38</v>
@@ -1718,7 +1591,7 @@
         <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>38</v>
@@ -1738,7 +1611,7 @@
         <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>38</v>
@@ -1758,7 +1631,7 @@
         <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>38</v>
@@ -1778,7 +1651,7 @@
         <v>44</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>45</v>
@@ -1798,7 +1671,7 @@
         <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>45</v>
@@ -1815,10 +1688,10 @@
         <v>43</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>47</v>
@@ -1838,7 +1711,7 @@
         <v>44</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>45</v>
@@ -1858,7 +1731,7 @@
         <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>45</v>
@@ -1875,10 +1748,10 @@
         <v>48</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>47</v>
@@ -1898,7 +1771,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>45</v>
@@ -1918,7 +1791,7 @@
         <v>46</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>45</v>
@@ -1935,10 +1808,10 @@
         <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>47</v>
@@ -1958,7 +1831,7 @@
         <v>51</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>45</v>
@@ -1978,7 +1851,7 @@
         <v>52</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>53</v>
@@ -1998,7 +1871,7 @@
         <v>44</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>45</v>
@@ -2018,7 +1891,7 @@
         <v>46</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>45</v>
@@ -2035,10 +1908,10 @@
         <v>54</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>47</v>
@@ -2058,7 +1931,7 @@
         <v>44</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>45</v>
@@ -2078,7 +1951,7 @@
         <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>45</v>
@@ -2095,10 +1968,10 @@
         <v>55</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>47</v>
@@ -2118,7 +1991,7 @@
         <v>44</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>45</v>
@@ -2138,7 +2011,7 @@
         <v>46</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>45</v>
@@ -2155,10 +2028,10 @@
         <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>47</v>
@@ -2178,7 +2051,7 @@
         <v>44</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>45</v>
@@ -2198,7 +2071,7 @@
         <v>46</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>45</v>
@@ -2215,10 +2088,10 @@
         <v>57</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>47</v>
@@ -2238,7 +2111,7 @@
         <v>44</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>45</v>
@@ -2258,7 +2131,7 @@
         <v>46</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>45</v>
@@ -2275,10 +2148,10 @@
         <v>58</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>47</v>
@@ -2298,7 +2171,7 @@
         <v>44</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>45</v>
@@ -2318,7 +2191,7 @@
         <v>46</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>45</v>
@@ -2335,10 +2208,10 @@
         <v>59</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>47</v>
@@ -2358,7 +2231,7 @@
         <v>62</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>45</v>
@@ -2378,7 +2251,7 @@
         <v>31</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>77</v>
@@ -2398,7 +2271,7 @@
         <v>31</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>77</v>
@@ -2418,7 +2291,7 @@
         <v>31</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>77</v>
@@ -2438,7 +2311,7 @@
         <v>31</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>82</v>
@@ -2458,7 +2331,7 @@
         <v>31</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>82</v>
@@ -2478,7 +2351,7 @@
         <v>31</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>82</v>
@@ -2498,7 +2371,7 @@
         <v>31</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>82</v>
@@ -2518,7 +2391,7 @@
         <v>31</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>82</v>
@@ -2538,7 +2411,7 @@
         <v>31</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>82</v>
@@ -2558,7 +2431,7 @@
         <v>89</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>53</v>
@@ -2578,7 +2451,7 @@
         <v>89</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>53</v>
@@ -2598,7 +2471,7 @@
         <v>89</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>53</v>
@@ -2618,7 +2491,7 @@
         <v>89</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>53</v>
@@ -2638,7 +2511,7 @@
         <v>89</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>53</v>
@@ -2658,7 +2531,7 @@
         <v>89</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>53</v>
@@ -2678,7 +2551,7 @@
         <v>89</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>53</v>
@@ -2698,7 +2571,7 @@
         <v>89</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>53</v>
@@ -2718,7 +2591,7 @@
         <v>89</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>53</v>
@@ -2738,7 +2611,7 @@
         <v>89</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>53</v>
@@ -2758,7 +2631,7 @@
         <v>90</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>47</v>
@@ -2778,7 +2651,7 @@
         <v>90</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>47</v>
@@ -2798,7 +2671,7 @@
         <v>90</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>47</v>
@@ -2818,7 +2691,7 @@
         <v>90</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>47</v>
@@ -2838,7 +2711,7 @@
         <v>90</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>47</v>
@@ -2858,7 +2731,7 @@
         <v>90</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>47</v>
@@ -2878,7 +2751,7 @@
         <v>90</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>47</v>
@@ -2898,7 +2771,7 @@
         <v>90</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>47</v>
@@ -2918,7 +2791,7 @@
         <v>90</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>47</v>
@@ -2938,7 +2811,7 @@
         <v>90</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>47</v>
@@ -2958,7 +2831,7 @@
         <v>89</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>53</v>
@@ -2978,7 +2851,7 @@
         <v>90</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>47</v>
@@ -2998,7 +2871,7 @@
         <v>93</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>38</v>
@@ -3018,7 +2891,7 @@
         <v>94</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>38</v>
@@ -3038,7 +2911,7 @@
         <v>89</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>53</v>
@@ -3058,7 +2931,7 @@
         <v>89</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>53</v>
@@ -3078,7 +2951,7 @@
         <v>89</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>53</v>
@@ -3098,7 +2971,7 @@
         <v>89</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>53</v>
@@ -3118,7 +2991,7 @@
         <v>89</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>53</v>
@@ -3138,7 +3011,7 @@
         <v>89</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>53</v>
@@ -3158,7 +3031,7 @@
         <v>89</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>53</v>
@@ -3178,7 +3051,7 @@
         <v>89</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>53</v>
@@ -3198,7 +3071,7 @@
         <v>89</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>53</v>
@@ -3218,7 +3091,7 @@
         <v>89</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>53</v>
@@ -3238,7 +3111,7 @@
         <v>90</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>47</v>
@@ -3258,7 +3131,7 @@
         <v>90</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>47</v>
@@ -3278,7 +3151,7 @@
         <v>90</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>47</v>
@@ -3298,7 +3171,7 @@
         <v>90</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>47</v>
@@ -3318,7 +3191,7 @@
         <v>90</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>47</v>
@@ -3338,7 +3211,7 @@
         <v>90</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>47</v>
@@ -3358,7 +3231,7 @@
         <v>90</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>47</v>
@@ -3378,7 +3251,7 @@
         <v>90</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>47</v>
@@ -3398,7 +3271,7 @@
         <v>90</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>47</v>
@@ -3418,7 +3291,7 @@
         <v>90</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>47</v>
@@ -3438,7 +3311,7 @@
         <v>37</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>38</v>
@@ -3458,7 +3331,7 @@
         <v>37</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>38</v>
@@ -3478,7 +3351,7 @@
         <v>39</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>38</v>
@@ -3498,7 +3371,7 @@
         <v>39</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>38</v>
@@ -3518,7 +3391,7 @@
         <v>37</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>38</v>
@@ -3538,7 +3411,7 @@
         <v>37</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>38</v>
@@ -3558,7 +3431,7 @@
         <v>39</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>38</v>
@@ -3578,7 +3451,7 @@
         <v>39</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>38</v>
@@ -3589,7 +3462,7 @@
         <v>11</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>63</v>
@@ -3598,10 +3471,10 @@
         <v>31</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
@@ -3609,7 +3482,7 @@
         <v>11</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>64</v>
@@ -3618,10 +3491,10 @@
         <v>31</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -3629,7 +3502,7 @@
         <v>11</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>65</v>
@@ -3638,10 +3511,10 @@
         <v>31</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -3649,7 +3522,7 @@
         <v>11</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>66</v>
@@ -3658,10 +3531,10 @@
         <v>31</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -3669,7 +3542,7 @@
         <v>11</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>67</v>
@@ -3678,10 +3551,10 @@
         <v>31</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -3689,7 +3562,7 @@
         <v>11</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>68</v>
@@ -3698,10 +3571,10 @@
         <v>31</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
@@ -3709,7 +3582,7 @@
         <v>11</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>69</v>
@@ -3718,10 +3591,10 @@
         <v>31</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
@@ -3729,7 +3602,7 @@
         <v>11</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>70</v>
@@ -3738,10 +3611,10 @@
         <v>31</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
@@ -3749,7 +3622,7 @@
         <v>11</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>71</v>
@@ -3758,10 +3631,10 @@
         <v>31</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
@@ -3769,7 +3642,7 @@
         <v>11</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>72</v>
@@ -3778,10 +3651,10 @@
         <v>31</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
@@ -3789,7 +3662,7 @@
         <v>11</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>73</v>
@@ -3798,10 +3671,10 @@
         <v>31</v>
       </c>
       <c r="E109" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F109" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3810,6 +3683,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e0782aab-51b8-4ca3-98ff-55b4e7f68941" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="33eab63c-ae56-4068-bee3-9f3b1109b8c5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009D19F62891C3BD42A3B191BFE4257989" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f702a18db7d267400f964a70eb93e56">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="33eab63c-ae56-4068-bee3-9f3b1109b8c5" xmlns:ns3="e0782aab-51b8-4ca3-98ff-55b4e7f68941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15fa389961bd8124ae695162c3af3829" ns2:_="" ns3:_="">
     <xsd:import namespace="33eab63c-ae56-4068-bee3-9f3b1109b8c5"/>
@@ -4058,17 +3942,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e0782aab-51b8-4ca3-98ff-55b4e7f68941" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="33eab63c-ae56-4068-bee3-9f3b1109b8c5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4079,6 +3952,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E416CA6D-4FD5-40FE-899F-FBEB9BE9EC31}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="e0782aab-51b8-4ca3-98ff-55b4e7f68941"/>
+    <ds:schemaRef ds:uri="33eab63c-ae56-4068-bee3-9f3b1109b8c5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{687CEDA3-8ED7-4B9A-8A23-5EF152B8A1F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4097,23 +3987,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E416CA6D-4FD5-40FE-899F-FBEB9BE9EC31}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="e0782aab-51b8-4ca3-98ff-55b4e7f68941"/>
-    <ds:schemaRef ds:uri="33eab63c-ae56-4068-bee3-9f3b1109b8c5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CE1014F-E953-4C02-A404-BD3BED220A6B}">
   <ds:schemaRefs>

</xml_diff>